<commit_message>
tạo danh sách thực tập, danh sách sv đăng ký và đồng bộ sever
</commit_message>
<xml_diff>
--- a/CSDL.xlsx
+++ b/CSDL.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="63">
   <si>
     <t>id</t>
   </si>
@@ -80,9 +80,6 @@
     <t>date</t>
   </si>
   <si>
-    <t>bit</t>
-  </si>
-  <si>
     <t>phone</t>
   </si>
   <si>
@@ -107,9 +104,6 @@
     <t>id_internship_type</t>
   </si>
   <si>
-    <t>id_course</t>
-  </si>
-  <si>
     <t>class</t>
   </si>
   <si>
@@ -207,6 +201,18 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>content</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>mssv</t>
+  </si>
+  <si>
+    <t>msgv</t>
   </si>
 </sst>
 </file>
@@ -289,11 +295,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -517,14 +524,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>493059</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>11206</xdr:rowOff>
+      <xdr:colOff>504265</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>504265</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>22412</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -533,9 +540,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7631206" y="4392706"/>
-          <a:ext cx="11206" cy="392206"/>
+        <a:xfrm flipH="1">
+          <a:off x="7648015" y="4572000"/>
+          <a:ext cx="3735" cy="212912"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -755,53 +762,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>605118</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>605118</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>22412</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="93" name="Straight Arrow Connector 92"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3541059" y="3238500"/>
-          <a:ext cx="0" cy="1546412"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="accent2"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent2"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>593912</xdr:colOff>
       <xdr:row>23</xdr:row>
@@ -875,8 +835,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="4930588" y="1669677"/>
-          <a:ext cx="2207559" cy="22412"/>
+          <a:off x="4933079" y="1669677"/>
+          <a:ext cx="2210671" cy="22412"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1218,25 +1178,20 @@
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent3"/>
-          </a:solidFill>
-          <a:prstDash val="dash"/>
-          <a:round/>
+        <a:ln>
           <a:headEnd type="none" w="med" len="med"/>
-          <a:tailEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="arrow" w="med" len="med"/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent3"/>
         </a:lnRef>
         <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
+          <a:schemeClr val="accent3"/>
         </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent3"/>
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="tx1"/>
@@ -1513,8 +1468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1535,14 +1490,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="6"/>
-      <c r="K2" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="L2" s="5"/>
+      <c r="I2" s="7"/>
+      <c r="K2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" s="6"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H3" s="1" t="s">
@@ -1552,7 +1507,7 @@
         <v>1</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>1</v>
@@ -1573,15 +1528,15 @@
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="6"/>
+      <c r="C5" s="7"/>
       <c r="H5" s="1" t="s">
-        <v>2</v>
+        <v>62</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>4</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
@@ -1592,19 +1547,19 @@
         <v>1</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K6" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="L6" s="6"/>
-      <c r="N6" s="6" t="s">
+      <c r="K6" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="O6" s="6"/>
+      <c r="L6" s="7"/>
+      <c r="N6" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="O6" s="7"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
@@ -1614,7 +1569,7 @@
         <v>4</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>4</v>
@@ -1626,7 +1581,7 @@
         <v>1</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>1</v>
@@ -1634,29 +1589,29 @@
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="5"/>
+      <c r="F8" s="6"/>
       <c r="H8" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>1</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>1</v>
@@ -1670,13 +1625,13 @@
         <v>1</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="L9" s="3" t="s">
         <v>1</v>
@@ -1687,10 +1642,10 @@
         <v>7</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>13</v>
@@ -1703,16 +1658,22 @@
       <c r="F11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="K11" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="L11" s="5"/>
+      <c r="H11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L11" s="6"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="5"/>
+      <c r="C12" s="6"/>
       <c r="E12" s="1" t="s">
         <v>12</v>
       </c>
@@ -1735,12 +1696,12 @@
       <c r="C13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H13" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I13" s="6"/>
+      <c r="H13" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I13" s="7"/>
       <c r="K13" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>1</v>
@@ -1767,62 +1728,52 @@
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E15" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F15" s="6"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
       <c r="H15" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="H16" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="L15" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E17" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
       <c r="H17" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K17" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="L17" s="6"/>
+      <c r="K17" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="L17" s="7"/>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="6"/>
+      <c r="C18" s="7"/>
       <c r="H18" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>4</v>
@@ -1842,10 +1793,10 @@
         <v>1</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>2</v>
@@ -1854,7 +1805,7 @@
         <v>4</v>
       </c>
       <c r="O19" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
@@ -1865,50 +1816,62 @@
         <v>4</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="H21" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>19</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="H22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="K22" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="L22" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B23" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="7"/>
+      <c r="K23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L23" s="1" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B23" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" s="6"/>
-      <c r="K23" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="L23" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
@@ -1918,6 +1881,12 @@
       <c r="C24" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="K24" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
@@ -1926,6 +1895,12 @@
       <c r="C25" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="K25" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
@@ -1934,14 +1909,10 @@
       <c r="C26" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E26" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F26" s="6"/>
-      <c r="K26" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="L26" s="5"/>
+      <c r="E26" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F26" s="7"/>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
@@ -1958,58 +1929,56 @@
       </c>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
-      <c r="K27" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L27" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="K27" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="L27" s="6"/>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>1</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="L28" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="N28" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="O28" s="5"/>
+      <c r="N28" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="O28" s="6"/>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>1</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="L29" s="1" t="s">
         <v>1</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="O29" s="1" t="s">
         <v>1</v>
@@ -2017,19 +1986,19 @@
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.25">
       <c r="E30" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="L30" s="1" t="s">
         <v>1</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="O30" s="1" t="s">
         <v>1</v>
@@ -2037,19 +2006,22 @@
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.25">
       <c r="E31" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="H31" t="s">
+        <v>58</v>
+      </c>
       <c r="K31" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="L31" s="1" t="s">
         <v>1</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="O31" s="1" t="s">
         <v>4</v>
@@ -2057,13 +2029,19 @@
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.25">
       <c r="E32" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="O32" s="1" t="s">
         <v>4</v>
@@ -2071,13 +2049,13 @@
     </row>
     <row r="33" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E33" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="O33" s="1" t="s">
         <v>1</v>
@@ -2085,13 +2063,13 @@
     </row>
     <row r="34" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E34" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="O34" s="1" t="s">
         <v>1</v>
@@ -2099,13 +2077,13 @@
     </row>
     <row r="35" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E35" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O35" s="1" t="s">
         <v>13</v>
@@ -2113,23 +2091,22 @@
     </row>
     <row r="36" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E36" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="15">
     <mergeCell ref="N28:O28"/>
     <mergeCell ref="N6:O6"/>
     <mergeCell ref="K6:L6"/>
     <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E15:F15"/>
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="K11:L11"/>
     <mergeCell ref="K17:L17"/>
-    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="K27:L27"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="B12:C12"/>
@@ -2139,6 +2116,7 @@
     <mergeCell ref="H13:I13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
client: sửa route - sửa QL thực tập
</commit_message>
<xml_diff>
--- a/CSDL.xlsx
+++ b/CSDL.xlsx
@@ -1468,8 +1468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2099,6 +2099,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B23:C23"/>
     <mergeCell ref="N28:O28"/>
     <mergeCell ref="N6:O6"/>
     <mergeCell ref="K6:L6"/>
@@ -2107,11 +2112,6 @@
     <mergeCell ref="K11:L11"/>
     <mergeCell ref="K17:L17"/>
     <mergeCell ref="K27:L27"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B23:C23"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="H13:I13"/>
   </mergeCells>

</xml_diff>

<commit_message>
update Hồ sơ đăng nhập
- Chức vụ giảng viên
- Doanh nghiệp đăng ký
- Sinh viên đăng ký
</commit_message>
<xml_diff>
--- a/CSDL.xlsx
+++ b/CSDL.xlsx
@@ -301,13 +301,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1468,8 +1468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1490,14 +1490,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="7"/>
-      <c r="K2" s="5" t="s">
+      <c r="I2" s="5"/>
+      <c r="K2" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="L2" s="6"/>
+      <c r="L2" s="7"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H3" s="1" t="s">
@@ -1528,10 +1528,10 @@
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="7"/>
+      <c r="C5" s="5"/>
       <c r="H5" s="1" t="s">
         <v>62</v>
       </c>
@@ -1552,14 +1552,14 @@
       <c r="I6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K6" s="7" t="s">
+      <c r="K6" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="L6" s="7"/>
-      <c r="N6" s="7" t="s">
+      <c r="L6" s="5"/>
+      <c r="N6" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="O6" s="7"/>
+      <c r="O6" s="5"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
@@ -1594,10 +1594,10 @@
       <c r="C8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="6"/>
+      <c r="F8" s="7"/>
       <c r="H8" s="1" t="s">
         <v>20</v>
       </c>
@@ -1642,7 +1642,7 @@
         <v>7</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>44</v>
@@ -1664,16 +1664,16 @@
       <c r="I11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K11" s="5" t="s">
+      <c r="K11" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="L11" s="6"/>
+      <c r="L11" s="7"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="6"/>
+      <c r="C12" s="7"/>
       <c r="E12" s="1" t="s">
         <v>12</v>
       </c>
@@ -1696,10 +1696,10 @@
       <c r="C13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H13" s="7" t="s">
+      <c r="H13" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="I13" s="7"/>
+      <c r="I13" s="5"/>
       <c r="K13" s="1" t="s">
         <v>38</v>
       </c>
@@ -1762,16 +1762,16 @@
       <c r="I17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K17" s="7" t="s">
+      <c r="K17" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="L17" s="7"/>
+      <c r="L17" s="5"/>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="7"/>
+      <c r="C18" s="5"/>
       <c r="H18" s="1" t="s">
         <v>26</v>
       </c>
@@ -1863,10 +1863,10 @@
       </c>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="7"/>
+      <c r="C23" s="5"/>
       <c r="K23" s="1" t="s">
         <v>20</v>
       </c>
@@ -1909,10 +1909,10 @@
       <c r="C26" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E26" s="7" t="s">
+      <c r="E26" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F26" s="7"/>
+      <c r="F26" s="5"/>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
@@ -1929,10 +1929,10 @@
       </c>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
-      <c r="K27" s="5" t="s">
+      <c r="K27" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="L27" s="6"/>
+      <c r="L27" s="7"/>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
@@ -1953,10 +1953,10 @@
       <c r="L28" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="N28" s="5" t="s">
+      <c r="N28" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="O28" s="6"/>
+      <c r="O28" s="7"/>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
@@ -2099,11 +2099,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B23:C23"/>
     <mergeCell ref="N28:O28"/>
     <mergeCell ref="N6:O6"/>
     <mergeCell ref="K6:L6"/>
@@ -2114,6 +2109,11 @@
     <mergeCell ref="K27:L27"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="H13:I13"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B23:C23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>